<commit_message>
Add print maven coordinates task
</commit_message>
<xml_diff>
--- a/gradle-maven-scopes.xlsx
+++ b/gradle-maven-scopes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artemptushkin/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/artemptushkin/JavaProjects/gradle-maven-scopes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B772C33-D3FE-4246-8C66-2E927D8ABBF6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E08FC09B-0B90-AA46-AB67-9F1C9653F276}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="35840" windowHeight="19240" xr2:uid="{FEC50B19-3640-3A4A-8403-41AECACC2DEE}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="30720" windowHeight="17140" xr2:uid="{FEC50B19-3640-3A4A-8403-41AECACC2DEE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="30">
   <si>
     <t>Gradle configurations</t>
   </si>
@@ -110,9 +110,6 @@
     <t>+</t>
   </si>
   <si>
-    <t>Included in Artifact?</t>
-  </si>
-  <si>
     <t>no</t>
   </si>
   <si>
@@ -123,6 +120,9 @@
   </si>
   <si>
     <t>Current artifact</t>
+  </si>
+  <si>
+    <t>Artifact inclusion</t>
   </si>
 </sst>
 </file>
@@ -158,7 +158,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -166,6 +166,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -480,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8064F04A-CEBC-5F44-B4E3-4F9B6D5B0B89}">
-  <dimension ref="A1:J13"/>
+  <dimension ref="A1:K13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J13" sqref="A1:J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -491,28 +492,29 @@
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="20" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.33203125" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="20" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.33203125" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="D1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="E1" s="2"/>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>28</v>
+      </c>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I1" s="2"/>
+      <c r="H1" s="2"/>
+      <c r="I1" s="2" t="s">
+        <v>27</v>
+      </c>
       <c r="J1" s="2"/>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="K1" s="3"/>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -523,28 +525,28 @@
         <v>14</v>
       </c>
       <c r="D2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" t="s">
         <v>20</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>21</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>22</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>23</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="I2" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="J2" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="J2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -552,7 +554,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>24</v>
@@ -563,15 +565,15 @@
       <c r="G3" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H3" s="1"/>
-      <c r="I3" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1"/>
       <c r="J3" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>4</v>
       </c>
@@ -582,7 +584,7 @@
         <v>15</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>24</v>
@@ -600,10 +602,10 @@
         <v>24</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -611,7 +613,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>24</v>
@@ -629,10 +631,10 @@
         <v>24</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -640,41 +642,41 @@
         <v>10</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="1"/>
       <c r="I6" s="1"/>
-      <c r="J6" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H7" s="1"/>
-      <c r="I7" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="D7" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I7" s="1"/>
       <c r="J7" s="1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>16</v>
       </c>
@@ -685,7 +687,7 @@
         <v>19</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>24</v>
@@ -696,13 +698,13 @@
       <c r="G8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J8" s="1"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>17</v>
       </c>
@@ -712,95 +714,103 @@
       <c r="C9" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="J9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="1"/>
+      <c r="D10" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E10" s="1"/>
-      <c r="F10" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="F10" s="1"/>
       <c r="G10" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E11" s="1"/>
-      <c r="F11" s="1" t="s">
-        <v>24</v>
-      </c>
+      <c r="F11" s="1"/>
       <c r="G11" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1"/>
-      <c r="F12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="G12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="1"/>
+      <c r="G12" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="H12" s="1"/>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
-      <c r="G13" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>24</v>
+      </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="H1:J1"/>
-    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="E1:H1"/>
+    <mergeCell ref="I1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>

</xml_diff>